<commit_message>
travel map - rating charts
</commit_message>
<xml_diff>
--- a/PROJECTS/Travel/Travel_map.xlsx
+++ b/PROJECTS/Travel/Travel_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb775b60f7163cde/Desktop/DATASET/TRAVEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb775b60f7163cde/Desktop/PYTHON FOR DATA ANALYSIS/PROJECTS/Travel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="8_{C7F799FC-F0C8-448E-9529-A38986D178C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A319F766-A4A6-4003-A453-F0F677249087}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B3EBFDF3-D941-40F5-8140-96606B3D392B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69396DBC-6E16-417E-BF1E-91BF537760CE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{CCD56015-54D0-400A-B01B-96F9E7F242B4}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>United Arab Emirates</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
     <t>Switzerland</t>
   </si>
   <si>
@@ -226,9 +220,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Undecided</t>
-  </si>
-  <si>
     <t>Caucasia</t>
   </si>
   <si>
@@ -248,6 +239,15 @@
   </si>
   <si>
     <t>Very safe</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Indifferent</t>
   </si>
 </sst>
 </file>
@@ -300,6 +300,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,7 +606,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,48 +622,48 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>40.409300000000002</v>
@@ -668,13 +672,13 @@
         <v>49.867100000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -683,18 +687,18 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>47.497900000000001</v>
@@ -703,13 +707,13 @@
         <v>19.040199999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -718,18 +722,18 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>50.075499999999998</v>
@@ -738,7 +742,7 @@
         <v>14.437799999999999</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -753,18 +757,18 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>46.947899999999997</v>
@@ -773,13 +777,13 @@
         <v>7.4474</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -788,18 +792,18 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>35.6892</v>
@@ -808,7 +812,7 @@
         <v>51.389000000000003</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -817,24 +821,24 @@
         <v>5</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>24.453900000000001</v>
@@ -843,7 +847,7 @@
         <v>54.377299999999998</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -858,18 +862,18 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>41.008200000000002</v>
@@ -878,7 +882,7 @@
         <v>28.978400000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -887,24 +891,24 @@
         <v>5</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>-37.813600000000001</v>
@@ -913,7 +917,7 @@
         <v>144.9631</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -928,18 +932,18 @@
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>8.5241000000000007</v>
@@ -948,33 +952,33 @@
         <v>76.936599999999999</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="H10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>1.3521000000000001</v>
@@ -983,10 +987,10 @@
         <v>103.8198</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -998,18 +1002,18 @@
         <v>3</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>-8.3405000000000005</v>
@@ -1018,7 +1022,7 @@
         <v>115.092</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G12">
         <v>4</v>
@@ -1033,18 +1037,18 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>13.7563</v>
@@ -1053,13 +1057,13 @@
         <v>100.5018</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G13">
         <v>4</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1068,18 +1072,18 @@
         <v>5</v>
       </c>
       <c r="K13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>42.697699999999998</v>
@@ -1088,7 +1092,7 @@
         <v>23.321899999999999</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G14">
         <v>4</v>
@@ -1100,21 +1104,21 @@
         <v>2</v>
       </c>
       <c r="J14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>44.4268</v>
@@ -1123,13 +1127,13 @@
         <v>26.102499999999999</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -1138,18 +1142,18 @@
         <v>3</v>
       </c>
       <c r="K15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <v>52.52</v>
@@ -1158,10 +1162,10 @@
         <v>13.404999999999999</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1173,18 +1177,18 @@
         <v>3</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>48.8566</v>
@@ -1193,13 +1197,13 @@
         <v>2.3521999999999998</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G17">
         <v>4</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I17">
         <v>5</v>
@@ -1208,13 +1212,25 @@
         <v>4</v>
       </c>
       <c r="K17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
     <sortCondition ref="A2:A17"/>
   </sortState>
+  <conditionalFormatting sqref="G2:K17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1238,16 +1254,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
@@ -1255,16 +1271,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
@@ -1272,16 +1288,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -1289,13 +1305,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
@@ -1303,13 +1319,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rating countries visited (plotly) + Beautify Folium map
</commit_message>
<xml_diff>
--- a/PROJECTS/Travel/Travel_map.xlsx
+++ b/PROJECTS/Travel/Travel_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb775b60f7163cde/Desktop/PYTHON FOR DATA ANALYSIS/PROJECTS/Travel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B3EBFDF3-D941-40F5-8140-96606B3D392B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69396DBC-6E16-417E-BF1E-91BF537760CE}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{853A51AD-0CFD-49E9-AE62-82292EDE26D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24F9CD18-9FD3-4099-AA7F-F4E9911E3A33}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{CCD56015-54D0-400A-B01B-96F9E7F242B4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t>Countries</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>Indifferent</t>
+  </si>
+  <si>
+    <t>Region_General</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
 </sst>
 </file>
@@ -300,10 +309,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -603,222 +608,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CE968A-5676-4958-B304-017DBDDF29E2}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="10.6328125" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" customWidth="1"/>
-    <col min="14" max="14" width="13.08984375" customWidth="1"/>
+    <col min="1" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" customWidth="1"/>
+    <col min="12" max="12" width="10.6328125" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
+    <col min="15" max="15" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>61</v>
       </c>
       <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>40.409300000000002</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>49.867100000000001</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
       <c r="H2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>47.497900000000001</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>19.040199999999999</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>49</v>
       </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
       <c r="H3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>50.075499999999998</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>14.437799999999999</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>49</v>
       </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
       <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
       <c r="J4">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>46.947899999999997</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>7.4474</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>49</v>
       </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>35.6892</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>51.389000000000003</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
       <c r="H6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>5</v>
@@ -826,400 +846,436 @@
       <c r="J6">
         <v>5</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>24.453900000000001</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>54.377299999999998</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
       <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
         <v>2</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>41.008200000000002</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>28.978400000000001</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>49</v>
       </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
       <c r="H8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8">
         <v>5</v>
       </c>
       <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>-37.813600000000001</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>144.9631</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>51</v>
       </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
       <c r="H9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>5</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>8.5241000000000007</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>76.936599999999999</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>2</v>
       </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
       <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
         <v>1.3521000000000001</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>103.8198</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>50</v>
       </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
       <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
         <v>2</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>-8.3405000000000005</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>115.092</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>49</v>
       </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
       <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
         <v>5</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>13.7563</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>100.5018</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>49</v>
       </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
       <c r="H13">
         <v>4</v>
       </c>
       <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>5</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>37</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>42.697699999999998</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>23.321899999999999</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>49</v>
       </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
       <c r="H14">
         <v>4</v>
       </c>
       <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
         <v>2</v>
       </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>44.4268</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>26.102499999999999</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>49</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
       <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="J15">
-        <v>3</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>39</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>52.52</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>13.404999999999999</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>49</v>
       </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
       <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
         <v>1</v>
       </c>
-      <c r="I16">
-        <v>5</v>
-      </c>
       <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="K16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>48.8566</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>2.3521999999999998</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>51</v>
       </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
       <c r="H17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
         <v>5</v>
       </c>
-      <c r="J17">
-        <v>4</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
     <sortCondition ref="A2:A17"/>
   </sortState>
-  <conditionalFormatting sqref="G2:K17">
+  <conditionalFormatting sqref="H2:L17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>